<commit_message>
Updates to character list
</commit_message>
<xml_diff>
--- a/Pollination Grant_character list.xlsx
+++ b/Pollination Grant_character list.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A72EEB-F242-4196-B96F-F0B6FC0E3F04}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8088" windowHeight="6558" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="71">
   <si>
     <t>Organismal</t>
   </si>
@@ -178,12 +179,66 @@
   </si>
   <si>
     <t>height</t>
+  </si>
+  <si>
+    <t>LM</t>
+  </si>
+  <si>
+    <t>SEM</t>
+  </si>
+  <si>
+    <t>TEM</t>
+  </si>
+  <si>
+    <t>(feel free to collapse these into one list if you prefer)</t>
+  </si>
+  <si>
+    <t>grain size</t>
+  </si>
+  <si>
+    <t>pore size</t>
+  </si>
+  <si>
+    <t>pore depth</t>
+  </si>
+  <si>
+    <t>annulus width</t>
+  </si>
+  <si>
+    <t>annulus depth</t>
+  </si>
+  <si>
+    <t>presence/absence of operculum</t>
+  </si>
+  <si>
+    <t>exine ornamentation</t>
+  </si>
+  <si>
+    <t>physical pollen description</t>
+  </si>
+  <si>
+    <t>grain shape</t>
+  </si>
+  <si>
+    <t>pollen wall ultrastructure</t>
+  </si>
+  <si>
+    <t>depth of exine ornamentation</t>
+  </si>
+  <si>
+    <t>presence/absence of microchannels</t>
+  </si>
+  <si>
+    <t>size of microchannels</t>
+  </si>
+  <si>
+    <t>orientation of microchannels</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -494,293 +549,364 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="3" max="3" width="26.9453125" customWidth="1"/>
+    <col min="4" max="4" width="17.26171875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.3671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C11" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C22" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C24" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C25" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C26" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C29" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C30" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C31" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C32" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C33" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C34" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C35" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C36" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C37" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C38" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C39" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C40" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C41" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C42" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C43" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C44" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C45" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C46" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C47" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C48" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C49" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C50" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C51" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B53" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C54" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C55" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C56" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C57" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C58" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C59" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B61" t="s">
         <v>4</v>
+      </c>
+      <c r="C61" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C62" t="s">
+        <v>53</v>
+      </c>
+      <c r="D62" t="s">
+        <v>54</v>
+      </c>
+      <c r="E62" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C63" t="s">
+        <v>57</v>
+      </c>
+      <c r="D63" t="s">
+        <v>63</v>
+      </c>
+      <c r="E63" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C64" t="s">
+        <v>65</v>
+      </c>
+      <c r="D64" t="s">
+        <v>58</v>
+      </c>
+      <c r="E64" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="65" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C65" t="s">
+        <v>64</v>
+      </c>
+      <c r="D65" t="s">
+        <v>59</v>
+      </c>
+      <c r="E65" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="66" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C66" t="s">
+        <v>62</v>
+      </c>
+      <c r="D66" t="s">
+        <v>60</v>
+      </c>
+      <c r="E66" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="67" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D67" t="s">
+        <v>61</v>
+      </c>
+      <c r="E67" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>